<commit_message>
complete excelDriver, verifyResult can be sorted now
</commit_message>
<xml_diff>
--- a/BMW_IAT/resources/user.xlsx
+++ b/BMW_IAT/resources/user.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>CaseID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,34 +133,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>user.accountList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前用户第三方帐号列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>oGsKmsy5FvOg0Knw9zbqi3z4oA3Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220049</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不离不弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>user.accountList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取当前用户第三方帐号列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>oGsKmsy5FvOg0Knw9zbqi3z4oA3Q</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>220049</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不离不弃</t>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":8,"data":"系统繁忙，请稍后重试哦~（8）"}</t>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -172,36 +197,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NT</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>{"userId":220112,"userName":"下雨天","t":"ZUjMFC1QxA2dQMF06BT1bYVxhD2MJOwM9","userSecretKey":"8ef1f70720cbdcbc0c4c1bcfeeac07b5","tag":1,"regTime":1421396002076,"bonus":0,"balance":1800,"inviteCode":"PWPG","type":1}</t>
-  </si>
-  <si>
-    <t>expected:&lt;[2]&gt; but was:&lt;[1]&gt;</t>
-  </si>
-  <si>
-    <t>{"accountList":[{"userId":220062,"extUserId":"1EDA5014E930971855AA9B50B4D2C46C","platform":"qq","type":0,"bindTime":1422859231248},{"userId":220062,"extUserId":"oGsKms0G_IG6cvXk0sKje9sP89XU","extUserName":"青青的小树","extUserPic":"http://wx.qlogo.cn/mmopen/5SEL2IohavAfuqZyOYF05Hhawjib7eeiajDHkldZOiatXhmzicnbpSLDucTdM5ibMsgOhaGpUCXFkBpx6GXibmsP1DibAZI0AsOV91M/0","platform":"weixin","type":1,"bindTime":0}]}</t>
-  </si>
-  <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"userId":220112,"userName":"下雨天","t":"ZVzZQXlcyAGRUNAZhBDwLMQg1XTFdb1Bu","userSecretKey":"73c9fe8fe0d5606d827ac93381057e77","tag":1,"regTime":1421396002076,"bonus":0,"balance":1800,"inviteCode":"PWPG","type":1}</t>
-  </si>
-  <si>
-    <t>{"code":8,"data":"系统繁忙，请稍后重试哦~（8）"}</t>
-  </si>
-  <si>
-    <t>JSONObject["tag"] not found.</t>
+    <t>{"userId":220112,"userName":"下雨天","t":"ZUzIFCwVgVzNUNAdgAjoONAs2CmYJO1Fv","userSecretKey":"6b1d26502d40355a9c74414a749965c3","tag":1,"regTime":1421396002076,"bonus":0,"balance":1800,"inviteCode":"PWPG","type":1}</t>
+  </si>
+  <si>
+    <t>expected:&lt;[220112]&gt; but was:&lt;[8]&gt;</t>
+  </si>
+  <si>
+    <t>&gt;0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notnull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"userId":220112,"userName":"下雨天","t":"ZB2YFCwtuAGQPb1I1ADgBOwE8DWEMPgQ6","userSecretKey":"49269a210cc319a71082bba82adc2f76","tag":1,"regTime":1421396002076,"bonus":0,"balance":1800,"inviteCode":"PWPG","type":1}</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1126,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1216,10 +1226,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="42" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>39</v>
       </c>
       <c r="E4" s="53" t="s">
         <v>12</v>
@@ -1249,10 +1259,10 @@
       <c r="D5" s="43"/>
       <c r="E5" s="54"/>
       <c r="F5" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>9</v>
@@ -1297,7 +1307,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="46"/>
       <c r="F7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>19</v>
@@ -1320,10 +1330,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="53" t="s">
         <v>12</v>
@@ -1344,7 +1354,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="42" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="P8" s="39"/>
     </row>
@@ -1420,14 +1430,14 @@
     </row>
     <row r="12" spans="1:16" ht="34">
       <c r="A12" s="47" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E12" s="53" t="s">
         <v>12</v>
@@ -1448,11 +1458,9 @@
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
       <c r="O12" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="P12" s="39" t="s">
-        <v>47</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="P12" s="39"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="48"/>
@@ -1485,10 +1493,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
@@ -1507,10 +1515,10 @@
       <c r="D15" s="44"/>
       <c r="E15" s="46"/>
       <c r="F15" s="35" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1568,7 +1576,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+      <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -1587,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="45"/>
       <c r="D1" s="55"/>
@@ -1609,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="54"/>
       <c r="D2" s="57"/>
@@ -1665,13 +1673,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E4" s="53" t="s">
         <v>12</v>
@@ -1685,9 +1693,7 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="42" t="s">
-        <v>43</v>
-      </c>
+      <c r="O4" s="42"/>
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16">

</xml_diff>